<commit_message>
Re-organized the documentation folder, renamed the files for the CAD models to make more sense. Updated the communication protocol emulator to auto detect the com port for an arduino.
</commit_message>
<xml_diff>
--- a/docs/rfgridCommunicationProtocol/rfgridCommunicationProtocol.xlsx
+++ b/docs/rfgridCommunicationProtocol/rfgridCommunicationProtocol.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ONEDRIVE\dev\rfgrid-ECED4900\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ONEDRIVE\dev\rfgrid-ECED4900\docs\rfgridCommunicationProtocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE3321F-A51E-4334-9D29-06F308C11BB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FDE3321F-A51E-4334-9D29-06F308C11BB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A185D98-DA8D-4B1E-9B62-ADB8640FAE3F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -266,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,6 +375,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -833,9 +839,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -849,9 +852,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -943,9 +943,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -981,24 +978,6 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1008,34 +987,61 @@
     <xf numFmtId="0" fontId="4" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1360,7 +1366,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="B2" sqref="B2:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,85 +1378,85 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="69"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="70"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="72"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="79"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="78"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="82"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="80"/>
-      <c r="E5" s="81" t="s">
+      <c r="D5" s="68"/>
+      <c r="E5" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="84" t="s">
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="84"/>
-      <c r="K5" s="85"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="73"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="56" t="s">
+      <c r="G6" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="57" t="s">
+      <c r="H6" s="54" t="s">
         <v>33</v>
       </c>
       <c r="I6" s="9" t="s">
@@ -1464,87 +1470,87 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="58"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="60"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="57"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34"/>
-      <c r="B8" s="61" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="63"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="60"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="64" t="s">
+      <c r="E9" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="66"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="63"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="30"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="28"/>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="45" t="s">
         <v>26</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -1553,40 +1559,40 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="39"/>
+      <c r="J11" s="37"/>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="40"/>
+      <c r="J12" s="38"/>
       <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="29" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -1595,20 +1601,20 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="39"/>
+      <c r="J13" s="37"/>
       <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="7" t="s">
@@ -1619,20 +1625,20 @@
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="40"/>
+      <c r="J14" s="38"/>
       <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="29" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="8" t="s">
@@ -1645,20 +1651,20 @@
         <v>46</v>
       </c>
       <c r="I15" s="4"/>
-      <c r="J15" s="39"/>
+      <c r="J15" s="37"/>
       <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="46" t="s">
         <v>26</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1671,114 +1677,114 @@
         <v>44</v>
       </c>
       <c r="I16" s="5"/>
-      <c r="J16" s="40"/>
+      <c r="J16" s="38"/>
       <c r="K16" s="11"/>
     </row>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="42" t="s">
+      <c r="G17" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="17"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="16"/>
     </row>
     <row r="18" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="58"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="60"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="57"/>
     </row>
     <row r="19" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="73" t="s">
+      <c r="B19" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="74"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="75"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="66"/>
     </row>
     <row r="20" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E20" s="64" t="s">
+      <c r="E20" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="66"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="63"/>
     </row>
     <row r="21" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="G21" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="30"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="28"/>
     </row>
     <row r="22" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="29" t="s">
         <v>28</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -1793,16 +1799,16 @@
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -1817,16 +1823,16 @@
       <c r="K23" s="11"/>
     </row>
     <row r="24" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="29" t="s">
         <v>28</v>
       </c>
       <c r="F24" s="3" t="s">
@@ -1839,16 +1845,16 @@
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F25" s="7" t="s">
@@ -1865,16 +1871,16 @@
       <c r="K25" s="11"/>
     </row>
     <row r="26" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="29" t="s">
         <v>28</v>
       </c>
       <c r="F26" s="8" t="s">
@@ -1889,16 +1895,16 @@
       <c r="K26" s="12"/>
     </row>
     <row r="27" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F27" s="1" t="s">
@@ -1919,16 +1925,16 @@
       <c r="K27" s="11"/>
     </row>
     <row r="28" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="33" t="s">
+      <c r="E28" s="31" t="s">
         <v>51</v>
       </c>
       <c r="F28" s="13" t="s">
@@ -1937,10 +1943,10 @@
       <c r="G28" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="17"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>